<commit_message>
simulaciones de los diodos y comence transistor
</commit_message>
<xml_diff>
--- a/Ej1/Mediciones/Mediciones.xlsx
+++ b/Ej1/Mediciones/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\ITBA\7° Cuatrimestre\Electrónica 1\Trabajos Prácticos\Electro1_TP1\Ej1\Mediciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88741731-B5A9-4656-9447-7B686FECA4A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED797C4-23BD-4644-8155-F72F19CA4F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="8247" xr2:uid="{A579DD31-FA90-4CCD-83BB-14F3A1A82F77}"/>
   </bookViews>
@@ -2479,7 +2479,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>